<commit_message>
updated one spreadsheet for new height arg
Now uses multiplier of value in space type json file vs. a hard coded
value in feet.
</commit_message>
<xml_diff>
--- a/projects/dfg_test_m0_office_blend_b_lhs.xlsx
+++ b/projects/dfg_test_m0_office_blend_b_lhs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="2940" windowWidth="21210" windowHeight="2835" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="3000" windowWidth="21210" windowHeight="2775" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2547" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2546" uniqueCount="918">
   <si>
     <t>type</t>
   </si>
@@ -2227,12 +2227,6 @@
     <t>Depth of perimeter thermal zone</t>
   </si>
   <si>
-    <t>floor_to_floor_height</t>
-  </si>
-  <si>
-    <t>Floor to floor height</t>
-  </si>
-  <si>
     <t>aspect_ratio_ns_to_ew</t>
   </si>
   <si>
@@ -2794,7 +2788,13 @@
     <t>Each SpaceType on at Least One Story Advanced Form</t>
   </si>
   <si>
-    <t>NationalGrid office blend, primary bar end</t>
+    <t>floor_to_floor_multiplier</t>
+  </si>
+  <si>
+    <t>Floor to Floor Height Multiplier</t>
+  </si>
+  <si>
+    <t>NationalGrid office blend, primary bar end, small test of reg val and new height logic</t>
   </si>
 </sst>
 </file>
@@ -7020,7 +7020,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7056,7 +7056,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>437</v>
@@ -7067,7 +7067,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>457</v>
@@ -7078,13 +7078,13 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>470</v>
       </c>
@@ -7171,7 +7171,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>660</v>
@@ -7291,7 +7291,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="30">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>588</v>
@@ -7364,7 +7364,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7395,7 +7395,7 @@
         <v>648</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7418,10 +7418,10 @@
         <v>649</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7429,10 +7429,10 @@
         <v>649</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="D44" s="2"/>
     </row>
@@ -7464,7 +7464,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7562,7 +7562,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>11</v>
@@ -7627,13 +7627,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
@@ -7646,16 +7646,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -7664,16 +7664,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="J6" s="31"/>
     </row>
@@ -7682,16 +7682,16 @@
         <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I7" s="52" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J7" s="31"/>
     </row>
@@ -7700,16 +7700,16 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I8" s="52" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="J8" s="31"/>
     </row>
@@ -7718,13 +7718,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>233</v>
@@ -7782,7 +7782,7 @@
         <v>104</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7790,7 +7790,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>717</v>
@@ -7819,7 +7819,7 @@
         <v>618</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -7832,22 +7832,22 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>719</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="G15" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I15" s="4">
-        <v>0.54</v>
+        <v>0</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3">
@@ -7866,7 +7866,7 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -7874,7 +7874,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>720</v>
@@ -7893,17 +7893,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J17" s="31"/>
     </row>
@@ -7912,7 +7912,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C18" s="37" t="s">
         <v>717</v>
@@ -7941,7 +7941,7 @@
         <v>618</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -7957,13 +7957,13 @@
         <v>22</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E20" s="31" t="s">
         <v>719</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="G20" s="31" t="s">
         <v>619</v>
@@ -7988,7 +7988,7 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -7996,7 +7996,7 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>720</v>
@@ -8015,17 +8015,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J22" s="31"/>
     </row>
@@ -8034,7 +8034,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>717</v>
@@ -8063,7 +8063,7 @@
         <v>618</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -8079,13 +8079,13 @@
         <v>22</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E25" s="31" t="s">
         <v>719</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="G25" s="31" t="s">
         <v>619</v>
@@ -8110,7 +8110,7 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -8118,7 +8118,7 @@
         <v>21</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E26" s="31" t="s">
         <v>720</v>
@@ -8137,17 +8137,17 @@
         <v>21</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J27" s="31"/>
     </row>
@@ -8156,7 +8156,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C28" s="37" t="s">
         <v>717</v>
@@ -8185,7 +8185,7 @@
         <v>618</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -8201,13 +8201,13 @@
         <v>22</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>719</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="G30" s="31" t="s">
         <v>619</v>
@@ -8232,7 +8232,7 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -8240,7 +8240,7 @@
         <v>21</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="E31" s="31" t="s">
         <v>720</v>
@@ -8259,17 +8259,17 @@
         <v>21</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I32" s="31" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J32" s="31"/>
     </row>
@@ -8297,7 +8297,7 @@
         <v>21</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E34" s="31" t="s">
         <v>725</v>
@@ -8348,19 +8348,16 @@
         <v>21</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>729</v>
+        <v>916</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>728</v>
+        <v>915</v>
       </c>
       <c r="G36" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H36" s="31" t="s">
-        <v>658</v>
-      </c>
       <c r="I36" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J36" s="31"/>
     </row>
@@ -8369,10 +8366,10 @@
         <v>21</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G37" s="31" t="s">
         <v>619</v>
@@ -8387,16 +8384,16 @@
         <v>21</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="G38" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="J38" s="31"/>
     </row>
@@ -8405,13 +8402,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="37" t="s">
+        <v>835</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>836</v>
+      </c>
+      <c r="D39" s="37" t="s">
         <v>837</v>
-      </c>
-      <c r="C39" s="37" t="s">
-        <v>838</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>839</v>
       </c>
       <c r="E39" s="37" t="s">
         <v>68</v>
@@ -8424,10 +8421,10 @@
         <v>21</v>
       </c>
       <c r="D40" s="46" t="s">
+        <v>757</v>
+      </c>
+      <c r="E40" s="46" t="s">
         <v>759</v>
-      </c>
-      <c r="E40" s="46" t="s">
-        <v>761</v>
       </c>
       <c r="G40" s="31" t="s">
         <v>619</v>
@@ -8453,7 +8450,7 @@
         <v>0.5</v>
       </c>
       <c r="R40" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -8461,10 +8458,10 @@
         <v>21</v>
       </c>
       <c r="D41" s="46" t="s">
+        <v>758</v>
+      </c>
+      <c r="E41" s="46" t="s">
         <v>760</v>
-      </c>
-      <c r="E41" s="46" t="s">
-        <v>762</v>
       </c>
       <c r="G41" s="31" t="s">
         <v>619</v>
@@ -8490,7 +8487,7 @@
         <v>0.5</v>
       </c>
       <c r="R41" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="42" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8498,13 +8495,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E42" s="37" t="s">
         <v>68</v>
@@ -8517,10 +8514,10 @@
         <v>22</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="G43" s="31" t="s">
         <v>619</v>
@@ -8545,7 +8542,7 @@
       <c r="O43" s="3"/>
       <c r="Q43" s="39"/>
       <c r="R43" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="44" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8553,13 +8550,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="37" t="s">
+        <v>746</v>
+      </c>
+      <c r="C44" s="37" t="s">
         <v>748</v>
       </c>
-      <c r="C44" s="37" t="s">
-        <v>750</v>
-      </c>
       <c r="D44" s="37" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E44" s="37" t="s">
         <v>68</v>
@@ -8572,10 +8569,10 @@
         <v>22</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G45" s="31" t="s">
         <v>619</v>
@@ -8600,7 +8597,7 @@
       <c r="O45" s="3"/>
       <c r="Q45" s="39"/>
       <c r="R45" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="46" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8608,13 +8605,13 @@
         <v>1</v>
       </c>
       <c r="B46" s="37" t="s">
+        <v>745</v>
+      </c>
+      <c r="C46" s="37" t="s">
         <v>747</v>
       </c>
-      <c r="C46" s="37" t="s">
-        <v>749</v>
-      </c>
       <c r="D46" s="37" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E46" s="37" t="s">
         <v>68</v>
@@ -8627,10 +8624,10 @@
         <v>22</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G47" s="31" t="s">
         <v>619</v>
@@ -8655,7 +8652,7 @@
       <c r="O47" s="3"/>
       <c r="Q47" s="39"/>
       <c r="R47" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -8663,13 +8660,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="47" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C48" s="47" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D48" s="47" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E48" s="47" t="s">
         <v>68</v>
@@ -8683,13 +8680,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E49" s="37" t="s">
         <v>68</v>
@@ -8702,13 +8699,13 @@
         <v>1</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E50" s="37" t="s">
         <v>68</v>
@@ -8749,7 +8746,7 @@
         <v>619</v>
       </c>
       <c r="H52" s="31" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="I52" s="31">
         <v>0</v>
@@ -8768,13 +8765,13 @@
         <v>1</v>
       </c>
       <c r="B53" s="47" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C53" s="47" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D53" s="47" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E53" s="47" t="s">
         <v>68</v>
@@ -8788,10 +8785,10 @@
         <v>22</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="G54" s="31" t="s">
         <v>619</v>
@@ -8816,7 +8813,7 @@
       <c r="O54" s="3"/>
       <c r="Q54" s="39"/>
       <c r="R54" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -8824,10 +8821,10 @@
         <v>21</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E55" s="31" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="G55" s="31" t="s">
         <v>619</v>
@@ -8849,10 +8846,10 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="G56" s="31" t="s">
         <v>619</v>
@@ -8874,10 +8871,10 @@
         <v>21</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="G57" s="31" t="s">
         <v>619</v>
@@ -8899,13 +8896,13 @@
         <v>1</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E58" s="37" t="s">
         <v>68</v>
@@ -8918,10 +8915,10 @@
         <v>21</v>
       </c>
       <c r="D59" s="31" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="E59" s="31" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="G59" s="31" t="s">
         <v>619</v>
@@ -8943,13 +8940,13 @@
         <v>1</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>68</v>
@@ -8962,10 +8959,10 @@
         <v>22</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E61" s="31" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G61" s="31" t="s">
         <v>619</v>
@@ -8990,7 +8987,7 @@
       <c r="O61" s="3"/>
       <c r="Q61" s="39"/>
       <c r="R61" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="62" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8998,13 +8995,13 @@
         <v>1</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -9017,10 +9014,10 @@
         <v>22</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="E63" s="31" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="G63" s="31" t="s">
         <v>619</v>
@@ -9045,7 +9042,7 @@
       <c r="O63" s="3"/>
       <c r="Q63" s="39"/>
       <c r="R63" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="64" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9053,13 +9050,13 @@
         <v>1</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -9072,10 +9069,10 @@
         <v>22</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E65" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G65" s="31" t="s">
         <v>619</v>
@@ -9100,7 +9097,7 @@
       <c r="O65" s="3"/>
       <c r="Q65" s="39"/>
       <c r="R65" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="66" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9108,13 +9105,13 @@
         <v>1</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -9127,10 +9124,10 @@
         <v>22</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E67" s="31" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="G67" s="31" t="s">
         <v>619</v>
@@ -9155,7 +9152,7 @@
       <c r="O67" s="3"/>
       <c r="Q67" s="39"/>
       <c r="R67" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9163,13 +9160,13 @@
         <v>1</v>
       </c>
       <c r="B68" s="37" t="s">
+        <v>788</v>
+      </c>
+      <c r="C68" s="37" t="s">
         <v>790</v>
       </c>
-      <c r="C68" s="37" t="s">
-        <v>792</v>
-      </c>
       <c r="D68" s="37" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>
@@ -9182,10 +9179,10 @@
         <v>22</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E69" s="31" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="G69" s="31" t="s">
         <v>619</v>
@@ -9210,7 +9207,7 @@
       <c r="O69" s="3"/>
       <c r="Q69" s="39"/>
       <c r="R69" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="70" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9218,13 +9215,13 @@
         <v>1</v>
       </c>
       <c r="B70" s="37" t="s">
+        <v>781</v>
+      </c>
+      <c r="C70" s="37" t="s">
         <v>783</v>
       </c>
-      <c r="C70" s="37" t="s">
-        <v>785</v>
-      </c>
       <c r="D70" s="37" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E70" s="37" t="s">
         <v>68</v>
@@ -9237,10 +9234,10 @@
         <v>21</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E71" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="G71" s="31" t="s">
         <v>619</v>
@@ -9262,10 +9259,10 @@
         <v>21</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E72" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G72" s="31" t="s">
         <v>619</v>
@@ -9287,13 +9284,13 @@
         <v>1</v>
       </c>
       <c r="B73" s="37" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C73" s="37" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D73" s="37" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E73" s="37" t="s">
         <v>68</v>
@@ -9306,13 +9303,13 @@
         <v>1</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D74" s="37" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E74" s="37" t="s">
         <v>68</v>
@@ -9325,13 +9322,13 @@
         <v>1</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D75" s="37" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="E75" s="37" t="s">
         <v>68</v>
@@ -9344,13 +9341,13 @@
         <v>1</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C76" s="37" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D76" s="37" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="E76" s="37" t="s">
         <v>68</v>
@@ -9363,13 +9360,13 @@
         <v>1</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C77" s="37" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D77" s="37" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="E77" s="37" t="s">
         <v>68</v>
@@ -9382,13 +9379,13 @@
         <v>1</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D78" s="37" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E78" s="37" t="s">
         <v>68</v>
@@ -9401,13 +9398,13 @@
         <v>1</v>
       </c>
       <c r="B79" s="37" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="D79" s="37" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="E79" s="37" t="s">
         <v>68</v>
@@ -9420,13 +9417,13 @@
         <v>1</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C80" s="37" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D80" s="37" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="E80" s="37" t="s">
         <v>68</v>
@@ -9439,13 +9436,13 @@
         <v>1</v>
       </c>
       <c r="B81" s="37" t="s">
+        <v>806</v>
+      </c>
+      <c r="C81" s="37" t="s">
+        <v>807</v>
+      </c>
+      <c r="D81" s="37" t="s">
         <v>808</v>
-      </c>
-      <c r="C81" s="37" t="s">
-        <v>809</v>
-      </c>
-      <c r="D81" s="37" t="s">
-        <v>810</v>
       </c>
       <c r="E81" s="37" t="s">
         <v>68</v>
@@ -9458,13 +9455,13 @@
         <v>1</v>
       </c>
       <c r="B82" s="37" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="C82" s="37" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="D82" s="37" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E82" s="37" t="s">
         <v>68</v>
@@ -9477,10 +9474,10 @@
         <v>21</v>
       </c>
       <c r="D83" s="46" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E83" s="46" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="G83" s="31" t="s">
         <v>619</v>
@@ -9506,7 +9503,7 @@
         <v>0.5</v>
       </c>
       <c r="R83" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
@@ -9514,10 +9511,10 @@
         <v>21</v>
       </c>
       <c r="D84" s="46" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E84" s="46" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="G84" s="31" t="s">
         <v>619</v>
@@ -9543,7 +9540,7 @@
         <v>0.5</v>
       </c>
       <c r="R84" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
@@ -9551,10 +9548,10 @@
         <v>22</v>
       </c>
       <c r="D85" s="46" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E85" s="46" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="G85" s="31" t="s">
         <v>619</v>
@@ -9580,7 +9577,7 @@
         <v>0.5</v>
       </c>
       <c r="R85" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
@@ -9588,10 +9585,10 @@
         <v>22</v>
       </c>
       <c r="D86" s="46" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E86" s="46" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="G86" s="31" t="s">
         <v>619</v>
@@ -9617,7 +9614,7 @@
         <v>0.5</v>
       </c>
       <c r="R86" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="87" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9625,13 +9622,13 @@
         <v>1</v>
       </c>
       <c r="B87" s="37" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C87" s="37" t="s">
+        <v>842</v>
+      </c>
+      <c r="D87" s="37" t="s">
         <v>844</v>
-      </c>
-      <c r="D87" s="37" t="s">
-        <v>846</v>
       </c>
       <c r="E87" s="37" t="s">
         <v>233</v>
@@ -9916,7 +9913,7 @@
         <v>459</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="C2" s="44" t="s">
         <v>635</v>
@@ -9955,7 +9952,7 @@
         <v>627</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>640</v>
@@ -9994,7 +9991,7 @@
         <v>642</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>636</v>
@@ -10027,7 +10024,7 @@
         <v>643</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>637</v>
@@ -10060,7 +10057,7 @@
         <v>644</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>639</v>
@@ -10093,7 +10090,7 @@
         <v>645</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>638</v>
@@ -10833,14 +10830,14 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="C32" s="40"/>
       <c r="D32" s="40" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="40" t="s">

</xml_diff>

<commit_message>
added contents of test spreadsheet to create_jsons
Nick, this should be ready for you to try to run.
</commit_message>
<xml_diff>
--- a/projects/dfg_test_m0_office_blend_b_lhs.xlsx
+++ b/projects/dfg_test_m0_office_blend_b_lhs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="3000" windowWidth="21210" windowHeight="2775" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="3000" windowWidth="15375" windowHeight="2775" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -7027,7 +7027,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7298,7 +7298,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="30">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>588</v>
@@ -7470,8 +7470,8 @@
   <dimension ref="A1:Z141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <pane ySplit="3" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>